<commit_message>
tried to add slider for overtime services
</commit_message>
<xml_diff>
--- a/ShinyApp/data/program-services-overtime.xlsx
+++ b/ShinyApp/data/program-services-overtime.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4718B04B-6624-1F49-A26C-F0AF3BD00A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5B5BF3-ABBC-5A46-A57C-14D82C7658C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{344E601E-E52B-2348-A200-BF30BBE16936}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Grand Total (unduplicated)</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t>Residential</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long </t>
+  </si>
+  <si>
+    <t xml:space="preserve">can plot this and other in barplots </t>
+  </si>
+  <si>
+    <t xml:space="preserve">can plot other in barplots </t>
   </si>
 </sst>
 </file>
@@ -459,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92802FF7-7108-AC45-845A-CA3651F280BB}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,9 +482,11 @@
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
     <col min="2" max="2" width="32.1640625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" customWidth="1"/>
+    <col min="10" max="10" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -495,9 +509,14 @@
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -520,9 +539,8 @@
       <c r="H2" s="1">
         <v>151</v>
       </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="7">
         <v>20166</v>
@@ -545,9 +563,14 @@
       <c r="H3" s="6">
         <v>66</v>
       </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3" s="1">
+        <v>-77.461934897545703</v>
+      </c>
+      <c r="J3">
+        <v>38.982148393478099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="7">
         <v>20175</v>
@@ -570,9 +593,14 @@
       <c r="H4" s="6">
         <v>8</v>
       </c>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I4" s="6">
+        <v>-77.596948920029405</v>
+      </c>
+      <c r="J4">
+        <v>39.0689724907512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="7">
         <v>20176</v>
@@ -595,9 +623,14 @@
       <c r="H5" s="6">
         <v>19</v>
       </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5" s="6">
+        <v>-77.532089824838707</v>
+      </c>
+      <c r="J5">
+        <v>39.202430396687802</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
         <v>4</v>
@@ -622,8 +655,10 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
@@ -647,7 +682,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -672,7 +707,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="7">
         <v>20175</v>
@@ -695,9 +730,14 @@
       <c r="H9" s="6">
         <v>1</v>
       </c>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9" s="6">
+        <v>-77.596948920029405</v>
+      </c>
+      <c r="J9">
+        <v>39.0689724907512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="7">
         <v>20176</v>
@@ -720,9 +760,14 @@
       <c r="H10" s="6">
         <v>19</v>
       </c>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I10" s="6">
+        <v>-77.532089824838707</v>
+      </c>
+      <c r="J10">
+        <v>39.202430396687802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="7" t="s">
         <v>4</v>
@@ -747,7 +792,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -772,7 +817,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="7">
         <v>20166</v>
@@ -795,9 +840,14 @@
       <c r="H13" s="6">
         <v>0</v>
       </c>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I13" s="1">
+        <v>-77.461934897545703</v>
+      </c>
+      <c r="J13">
+        <v>38.982148393478099</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="7">
         <v>20175</v>
@@ -820,9 +870,14 @@
       <c r="H14" s="6">
         <v>3</v>
       </c>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14" s="6">
+        <v>-77.596948920029405</v>
+      </c>
+      <c r="J14">
+        <v>39.0689724907512</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="7">
         <v>20176</v>
@@ -845,9 +900,14 @@
       <c r="H15" s="6">
         <v>118</v>
       </c>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I15" s="6">
+        <v>-77.532089824838707</v>
+      </c>
+      <c r="J15">
+        <v>39.202430396687802</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="7" t="s">
         <v>4</v>
@@ -872,8 +932,10 @@
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B17" s="7" t="s">
         <v>5</v>
       </c>
@@ -897,7 +959,7 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
@@ -922,7 +984,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="7">
         <v>20175</v>
@@ -945,9 +1007,14 @@
       <c r="H19" s="6">
         <v>8</v>
       </c>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I19" s="6">
+        <v>-77.596948920029405</v>
+      </c>
+      <c r="J19">
+        <v>39.0689724907512</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="7" t="s">
         <v>4</v>
@@ -972,7 +1039,7 @@
       </c>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -997,7 +1064,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="7">
         <v>20166</v>
@@ -1020,9 +1087,14 @@
       <c r="H22" s="6">
         <v>56</v>
       </c>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="1">
+        <v>-77.461934897545703</v>
+      </c>
+      <c r="J22">
+        <v>38.982148393478099</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="7">
         <v>20175</v>
@@ -1045,9 +1117,14 @@
       <c r="H23" s="6">
         <v>15</v>
       </c>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="6">
+        <v>-77.596948920029405</v>
+      </c>
+      <c r="J23">
+        <v>39.0689724907512</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="7">
         <v>20176</v>
@@ -1070,9 +1147,14 @@
       <c r="H24" s="6">
         <v>112</v>
       </c>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I24" s="6">
+        <v>-77.532089824838707</v>
+      </c>
+      <c r="J24">
+        <v>39.202430396687802</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="7" t="s">
         <v>4</v>
@@ -1097,8 +1179,10 @@
       </c>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B26" s="7" t="s">
         <v>5</v>
       </c>
@@ -1122,7 +1206,7 @@
       </c>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1231,7 @@
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="7">
         <v>20132</v>
@@ -1170,9 +1254,14 @@
       <c r="H28" s="6">
         <v>0</v>
       </c>
-      <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I28" s="6">
+        <v>-77.723573692312499</v>
+      </c>
+      <c r="J28">
+        <v>39.169619032191399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="7">
         <v>20147</v>
@@ -1195,9 +1284,14 @@
       <c r="H29" s="6">
         <v>1</v>
       </c>
-      <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I29" s="6">
+        <v>-77.482812313593001</v>
+      </c>
+      <c r="J29">
+        <v>39.0419667639473</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="7">
         <v>20164</v>
@@ -1220,9 +1314,14 @@
       <c r="H30" s="6">
         <v>0</v>
       </c>
-      <c r="I30" s="6"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I30" s="6">
+        <v>-77.393658181930903</v>
+      </c>
+      <c r="J30">
+        <v>39.011138616915403</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="7">
         <v>20165</v>
@@ -1245,9 +1344,14 @@
       <c r="H31" s="6">
         <v>1</v>
       </c>
-      <c r="I31" s="6"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I31" s="6">
+        <v>-77.387517040821294</v>
+      </c>
+      <c r="J31">
+        <v>39.056421479138898</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="7">
         <v>20175</v>
@@ -1270,10 +1374,17 @@
       <c r="H32" s="6">
         <v>0</v>
       </c>
-      <c r="I32" s="6"/>
+      <c r="I32" s="6">
+        <v>-77.596948920029405</v>
+      </c>
+      <c r="J32">
+        <v>39.0689724907512</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
+      <c r="A33" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="B33" s="7" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
added in zip code outlines and circles corresponding to number of programs over time
</commit_message>
<xml_diff>
--- a/ShinyApp/data/program-services-overtime.xlsx
+++ b/ShinyApp/data/program-services-overtime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5B5BF3-ABBC-5A46-A57C-14D82C7658C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9A5FB3-4022-4E40-90A6-5D8235C3FD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{344E601E-E52B-2348-A200-BF30BBE16936}"/>
   </bookViews>
@@ -34,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Grand Total (unduplicated)</t>
   </si>
   <si>
     <t>Program &amp; Service Location Zip Code</t>
-  </si>
-  <si>
-    <t>2021 YTD</t>
   </si>
   <si>
     <t>Case Management</t>
@@ -72,13 +69,13 @@
     <t>Lat</t>
   </si>
   <si>
-    <t xml:space="preserve">Long </t>
-  </si>
-  <si>
     <t xml:space="preserve">can plot this and other in barplots </t>
   </si>
   <si>
     <t xml:space="preserve">can plot other in barplots </t>
+  </si>
+  <si>
+    <t>Long</t>
   </si>
 </sst>
 </file>
@@ -140,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -157,6 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +472,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,34 +489,34 @@
         <v>1</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1">
+      <c r="C1" s="8">
         <v>2016</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="8">
         <v>2017</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="8">
         <v>2018</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="8">
         <v>2019</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="8">
         <v>2020</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
+      <c r="H1" s="8">
+        <v>2021</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="1">
@@ -633,7 +631,7 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6">
         <v>82</v>
@@ -657,10 +655,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -684,7 +682,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="1">
@@ -770,7 +768,7 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="6">
         <v>13</v>
@@ -794,7 +792,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="1">
@@ -910,7 +908,7 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="6">
         <v>150</v>
@@ -934,10 +932,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="6">
         <v>0</v>
@@ -961,7 +959,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="1">
@@ -1017,7 +1015,7 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="6">
         <v>15</v>
@@ -1041,7 +1039,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="1">
@@ -1157,7 +1155,7 @@
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" s="6">
         <v>112</v>
@@ -1181,10 +1179,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="6">
         <v>0</v>
@@ -1208,7 +1206,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="1">
@@ -1383,10 +1381,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33" s="6">
         <v>3</v>

</xml_diff>